<commit_message>
fixed issue with curren$y sign
</commit_message>
<xml_diff>
--- a/FX Rates.xlsx
+++ b/FX Rates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrah\OneDrive\Documents\Fun programming code\Currency-Conversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrah\OneDrive\Documents\Fun programming code\CurrencyConversionJSApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81FFA0E-E96C-4C90-9B8E-EEB74CE39ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB56BBD4-07CD-43D8-B818-55E623DC2AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{D74C95F1-E3B4-4CB6-9AE4-F7BE63C64A25}"/>
   </bookViews>
@@ -1253,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDEE740-4797-4A50-B11C-2EFFEE281F27}">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1362,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="13">
-        <v>1.3888888888888888</v>
+        <v>1.3888888888888899</v>
       </c>
       <c r="D6" s="13">
         <v>1.3888888888888888</v>

</xml_diff>

<commit_message>
fixed spaces in country issue with select option value
</commit_message>
<xml_diff>
--- a/FX Rates.xlsx
+++ b/FX Rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrah\OneDrive\Documents\Fun programming code\CurrencyConversionJSApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB56BBD4-07CD-43D8-B818-55E623DC2AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1324AFBB-560B-4A87-BFAF-C8E1910FD5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{D74C95F1-E3B4-4CB6-9AE4-F7BE63C64A25}"/>
   </bookViews>
@@ -1253,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDEE740-4797-4A50-B11C-2EFFEE281F27}">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>

</xml_diff>